<commit_message>
Últimas modificações na tabela
</commit_message>
<xml_diff>
--- a/DUMA.xlsx
+++ b/DUMA.xlsx
@@ -955,8 +955,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AW59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView tabSelected="1" topLeftCell="AB32" workbookViewId="0">
+      <selection activeCell="AJ48" sqref="AJ48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1442,7 +1442,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="17" spans="1:38">
+    <row r="17" spans="1:46">
       <c r="A17" t="s">
         <v>14</v>
       </c>
@@ -1492,7 +1492,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="18" spans="1:38">
+    <row r="18" spans="1:46">
       <c r="A18" t="s">
         <v>15</v>
       </c>
@@ -1518,7 +1518,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="19" spans="1:38">
+    <row r="19" spans="1:46">
       <c r="A19" t="s">
         <v>16</v>
       </c>
@@ -1544,7 +1544,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="20" spans="1:38">
+    <row r="20" spans="1:46">
       <c r="A20" t="s">
         <v>24</v>
       </c>
@@ -1567,7 +1567,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="21" spans="1:38">
+    <row r="21" spans="1:46">
       <c r="A21" t="s">
         <v>26</v>
       </c>
@@ -1595,14 +1595,14 @@
       <c r="U21" t="s">
         <v>121</v>
       </c>
-      <c r="AJ21" t="s">
-        <v>121</v>
-      </c>
       <c r="AK21" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="22" spans="1:38">
+      <c r="AT21" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="22" spans="1:46">
       <c r="A22" t="s">
         <v>27</v>
       </c>
@@ -1610,7 +1610,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="23" spans="1:38">
+    <row r="23" spans="1:46">
       <c r="A23" t="s">
         <v>28</v>
       </c>
@@ -1633,7 +1633,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="24" spans="1:38">
+    <row r="24" spans="1:46">
       <c r="A24" t="s">
         <v>29</v>
       </c>
@@ -1653,7 +1653,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="25" spans="1:38">
+    <row r="25" spans="1:46">
       <c r="A25" t="s">
         <v>30</v>
       </c>
@@ -1664,7 +1664,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="26" spans="1:38">
+    <row r="26" spans="1:46">
       <c r="A26" t="s">
         <v>25</v>
       </c>
@@ -1672,7 +1672,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="27" spans="1:38">
+    <row r="27" spans="1:46">
       <c r="A27" t="s">
         <v>31</v>
       </c>
@@ -1698,7 +1698,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="28" spans="1:38">
+    <row r="28" spans="1:46">
       <c r="A28" t="s">
         <v>32</v>
       </c>
@@ -1709,7 +1709,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="29" spans="1:38">
+    <row r="29" spans="1:46">
       <c r="A29" t="s">
         <v>33</v>
       </c>
@@ -1732,7 +1732,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="30" spans="1:38">
+    <row r="30" spans="1:46">
       <c r="A30" t="s">
         <v>17</v>
       </c>
@@ -1740,7 +1740,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="31" spans="1:38">
+    <row r="31" spans="1:46">
       <c r="A31" t="s">
         <v>34</v>
       </c>
@@ -1754,7 +1754,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="32" spans="1:38">
+    <row r="32" spans="1:46">
       <c r="A32" t="s">
         <v>35</v>
       </c>
@@ -2043,10 +2043,10 @@
       <c r="U44" t="s">
         <v>173</v>
       </c>
-      <c r="AJ44" t="s">
+      <c r="AK44" t="s">
         <v>173</v>
       </c>
-      <c r="AK44" t="s">
+      <c r="AT44" t="s">
         <v>173</v>
       </c>
     </row>
@@ -2092,10 +2092,10 @@
       <c r="U46" t="s">
         <v>145</v>
       </c>
-      <c r="AJ46" t="s">
+      <c r="AK46" t="s">
         <v>145</v>
       </c>
-      <c r="AK46" t="s">
+      <c r="AT46" t="s">
         <v>145</v>
       </c>
     </row>
@@ -2144,10 +2144,10 @@
       <c r="U48" t="s">
         <v>147</v>
       </c>
-      <c r="AJ48" t="s">
+      <c r="AK48" t="s">
         <v>147</v>
       </c>
-      <c r="AK48" t="s">
+      <c r="AT48" t="s">
         <v>147</v>
       </c>
     </row>
@@ -2199,10 +2199,10 @@
       <c r="U50" t="s">
         <v>180</v>
       </c>
-      <c r="AJ50" t="s">
+      <c r="AK50" t="s">
         <v>180</v>
       </c>
-      <c r="AK50" t="s">
+      <c r="AT50" t="s">
         <v>180</v>
       </c>
     </row>
@@ -2257,10 +2257,10 @@
       <c r="U52" t="s">
         <v>183</v>
       </c>
-      <c r="AJ52" t="s">
+      <c r="AK52" t="s">
         <v>183</v>
       </c>
-      <c r="AK52" t="s">
+      <c r="AT52" t="s">
         <v>183</v>
       </c>
     </row>
@@ -2318,10 +2318,10 @@
       <c r="U54" t="s">
         <v>186</v>
       </c>
-      <c r="AJ54" t="s">
+      <c r="AK54" t="s">
         <v>186</v>
       </c>
-      <c r="AK54" t="s">
+      <c r="AT54" t="s">
         <v>186</v>
       </c>
     </row>

</xml_diff>